<commit_message>
looking at lazer more
</commit_message>
<xml_diff>
--- a/Lazar_data.xlsx
+++ b/Lazar_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kelseabest/Documents/Research/ABM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kelseabest/Documents/Research/ABM/ABM_py/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5208D3E4-C58C-A04F-8399-B7A6C5AAEB3D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EDDD60F-8968-8248-A29A-BAA8810DC75F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="13580" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20500" windowHeight="13080" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="5" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="82">
   <si>
     <t>Years</t>
   </si>
@@ -500,6 +500,9 @@
   </si>
   <si>
     <t>Modelling household well-being and poverty trajectories: an application to coastal Bangladesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1190,7 +1193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -15960,10 +15963,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:T112"/>
+  <dimension ref="A1:U112"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15988,12 +15991,12 @@
     <col min="19" max="20" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="10"/>
       <c r="C2" s="39" t="s">
@@ -16019,7 +16022,7 @@
       <c r="S2" s="43"/>
       <c r="T2" s="44"/>
     </row>
-    <row r="3" spans="1:20" ht="104" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="104" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>15</v>
       </c>
@@ -16081,7 +16084,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>28</v>
       </c>
@@ -16143,7 +16146,7 @@
         <v>4904</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>29</v>
       </c>
@@ -16205,7 +16208,7 @@
         <v>8192</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>30</v>
       </c>
@@ -16267,7 +16270,7 @@
         <v>12192</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>31</v>
       </c>
@@ -16329,7 +16332,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>32</v>
       </c>
@@ -16391,7 +16394,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>33</v>
       </c>
@@ -16453,7 +16456,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>34</v>
       </c>
@@ -16515,7 +16518,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>35</v>
       </c>
@@ -16577,7 +16580,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>36</v>
       </c>
@@ -16639,7 +16642,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>37</v>
       </c>
@@ -16701,7 +16704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>38</v>
       </c>
@@ -16762,8 +16765,11 @@
       <c r="T14" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>39</v>
       </c>
@@ -16825,7 +16831,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>40</v>
       </c>

</xml_diff>